<commit_message>
added : basic history tab on homepage
</commit_message>
<xml_diff>
--- a/public/data/db_source/institution.xlsx
+++ b/public/data/db_source/institution.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{217DAAA9-9EA2-194C-9218-8F5FA2D61494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B4222E7-E991-974F-A32F-9EEFFD23AE82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2940" yWindow="500" windowWidth="25860" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="235">
   <si>
     <t>id</t>
   </si>
@@ -747,6 +747,9 @@
   </si>
   <si>
     <t>population, societe, transport</t>
+  </si>
+  <si>
+    <t>021 692 11 11</t>
   </si>
 </sst>
 </file>
@@ -1131,10 +1134,10 @@
   <dimension ref="A1:I70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="168" zoomScaleNormal="170" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B54" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G20" sqref="G20"/>
+      <selection pane="bottomRight" activeCell="F72" sqref="F72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2112,7 +2115,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>211</v>
       </c>
@@ -2126,7 +2129,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>214</v>
       </c>
@@ -2140,7 +2143,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>217</v>
       </c>
@@ -2154,7 +2157,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>220</v>
       </c>
@@ -2168,7 +2171,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>223</v>
       </c>
@@ -2182,7 +2185,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>226</v>
       </c>
@@ -2194,6 +2197,9 @@
       </c>
       <c r="D70" s="1" t="s">
         <v>228</v>
+      </c>
+      <c r="F70" t="s">
+        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added : history tab to all pages
</commit_message>
<xml_diff>
--- a/public/data/db_source/institution.xlsx
+++ b/public/data/db_source/institution.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B4222E7-E991-974F-A32F-9EEFFD23AE82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96EF1ED4-61DA-4F4F-8F21-D3E4F92036F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2940" yWindow="500" windowWidth="25860" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="236">
   <si>
     <t>id</t>
   </si>
@@ -406,9 +406,6 @@
   </si>
   <si>
     <t>OCSTAT : Office Cantonal de la Statistique (GE)</t>
-  </si>
-  <si>
-    <t>L’Office cantonal de la statistique assure l’information statistique publique en mettant à disposition des autorités et de la collectivité dans son ensemble des informations statistiques pertinentes, fiables et cohérentes.</t>
   </si>
   <si>
     <t>statistique@etat.ge.ch</t>
@@ -750,6 +747,12 @@
   </si>
   <si>
     <t>021 692 11 11</t>
+  </si>
+  <si>
+    <t>L’Office cantonal de la statistique assure l’information statistique en mettant à disposition des autorités, du public et de la collectivité dans son ensemble des informations statistiques pertinentes, fiables et cohérentes.</t>
+  </si>
+  <si>
+    <t>test@email.ch</t>
   </si>
 </sst>
 </file>
@@ -785,11 +788,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1134,10 +1138,10 @@
   <dimension ref="A1:I70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="168" zoomScaleNormal="170" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B54" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C51" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F72" sqref="F72"/>
+      <selection pane="bottomRight" activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1172,10 +1176,10 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>228</v>
+      </c>
+      <c r="H1" t="s">
         <v>229</v>
-      </c>
-      <c r="H1" t="s">
-        <v>230</v>
       </c>
       <c r="I1" s="1"/>
     </row>
@@ -1190,7 +1194,7 @@
         <v>8</v>
       </c>
       <c r="H2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1499,10 +1503,10 @@
         <v>75</v>
       </c>
       <c r="G23" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H23" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1735,471 +1739,474 @@
         <v>125</v>
       </c>
       <c r="D39" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="E39" t="s">
         <v>126</v>
       </c>
-      <c r="E39" t="s">
+      <c r="F39" t="s">
         <v>127</v>
-      </c>
-      <c r="F39" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B40" t="s">
         <v>6</v>
       </c>
       <c r="C40" t="s">
+        <v>129</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
+        <v>131</v>
+      </c>
+      <c r="B41" t="s">
+        <v>128</v>
+      </c>
+      <c r="C41" t="s">
         <v>132</v>
       </c>
-      <c r="B41" t="s">
-        <v>129</v>
-      </c>
-      <c r="C41" t="s">
+      <c r="D41" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="E41" t="s">
         <v>134</v>
       </c>
-      <c r="E41" t="s">
+      <c r="F41" t="s">
         <v>135</v>
-      </c>
-      <c r="F41" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>136</v>
+      </c>
+      <c r="B42" t="s">
+        <v>131</v>
+      </c>
+      <c r="C42" t="s">
         <v>137</v>
       </c>
-      <c r="B42" t="s">
-        <v>132</v>
-      </c>
-      <c r="C42" t="s">
+      <c r="D42" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="E42" t="s">
         <v>139</v>
       </c>
-      <c r="E42" t="s">
+      <c r="F42" t="s">
         <v>140</v>
-      </c>
-      <c r="F42" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B43" t="s">
         <v>114</v>
       </c>
       <c r="C43" t="s">
+        <v>142</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B44" t="s">
         <v>114</v>
       </c>
       <c r="C44" t="s">
+        <v>145</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B45" t="s">
         <v>114</v>
       </c>
       <c r="C45" t="s">
+        <v>148</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B46" t="s">
         <v>114</v>
       </c>
       <c r="C46" t="s">
+        <v>151</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B47" t="s">
         <v>114</v>
       </c>
       <c r="C47" t="s">
+        <v>154</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B48" t="s">
         <v>114</v>
       </c>
       <c r="C48" t="s">
+        <v>157</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>158</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B49" t="s">
         <v>114</v>
       </c>
       <c r="C49" t="s">
+        <v>160</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="F49" t="s">
         <v>162</v>
-      </c>
-      <c r="F49" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B50" t="s">
         <v>114</v>
       </c>
       <c r="C50" t="s">
+        <v>164</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
+        <v>166</v>
+      </c>
+      <c r="B51" t="s">
+        <v>163</v>
+      </c>
+      <c r="C51" t="s">
         <v>167</v>
       </c>
-      <c r="B51" t="s">
-        <v>164</v>
-      </c>
-      <c r="C51" t="s">
+      <c r="D51" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
+        <v>169</v>
+      </c>
+      <c r="B52" t="s">
+        <v>166</v>
+      </c>
+      <c r="C52" t="s">
         <v>170</v>
       </c>
-      <c r="B52" t="s">
-        <v>167</v>
-      </c>
-      <c r="C52" t="s">
+      <c r="D52" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
+        <v>172</v>
+      </c>
+      <c r="B53" t="s">
+        <v>156</v>
+      </c>
+      <c r="C53" t="s">
         <v>173</v>
       </c>
-      <c r="B53" t="s">
-        <v>157</v>
-      </c>
-      <c r="C53" t="s">
+      <c r="D53" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
+        <v>175</v>
+      </c>
+      <c r="B54" t="s">
+        <v>147</v>
+      </c>
+      <c r="C54" t="s">
         <v>176</v>
       </c>
-      <c r="B54" t="s">
-        <v>148</v>
-      </c>
-      <c r="C54" t="s">
+      <c r="D54" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
+        <v>178</v>
+      </c>
+      <c r="B55" t="s">
+        <v>150</v>
+      </c>
+      <c r="C55" t="s">
         <v>179</v>
       </c>
-      <c r="B55" t="s">
-        <v>151</v>
-      </c>
-      <c r="C55" t="s">
+      <c r="D55" s="1" t="s">
         <v>180</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>181</v>
+      </c>
+      <c r="B56" t="s">
+        <v>178</v>
+      </c>
+      <c r="C56" t="s">
         <v>182</v>
       </c>
-      <c r="B56" t="s">
-        <v>179</v>
-      </c>
-      <c r="C56" t="s">
+      <c r="D56" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
+        <v>184</v>
+      </c>
+      <c r="B57" t="s">
+        <v>178</v>
+      </c>
+      <c r="C57" t="s">
         <v>185</v>
       </c>
-      <c r="B57" t="s">
-        <v>179</v>
-      </c>
-      <c r="C57" t="s">
+      <c r="D57" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
+        <v>187</v>
+      </c>
+      <c r="B58" t="s">
+        <v>153</v>
+      </c>
+      <c r="C58" t="s">
         <v>188</v>
       </c>
-      <c r="B58" t="s">
-        <v>154</v>
-      </c>
-      <c r="C58" t="s">
+      <c r="D58" s="1" t="s">
         <v>189</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
+        <v>190</v>
+      </c>
+      <c r="B59" t="s">
+        <v>144</v>
+      </c>
+      <c r="C59" t="s">
         <v>191</v>
       </c>
-      <c r="B59" t="s">
-        <v>145</v>
-      </c>
-      <c r="C59" t="s">
+      <c r="D59" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
+        <v>193</v>
+      </c>
+      <c r="B60" t="s">
+        <v>150</v>
+      </c>
+      <c r="C60" t="s">
         <v>194</v>
       </c>
-      <c r="B60" t="s">
-        <v>151</v>
-      </c>
-      <c r="C60" t="s">
+      <c r="D60" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
+        <v>196</v>
+      </c>
+      <c r="B61" t="s">
+        <v>159</v>
+      </c>
+      <c r="C61" t="s">
         <v>197</v>
       </c>
-      <c r="B61" t="s">
-        <v>160</v>
-      </c>
-      <c r="C61" t="s">
+      <c r="D61" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="D61" s="1" t="s">
+      <c r="E61" t="s">
         <v>199</v>
       </c>
-      <c r="E61" t="s">
+      <c r="F61" t="s">
         <v>200</v>
-      </c>
-      <c r="F61" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
+        <v>201</v>
+      </c>
+      <c r="B62" t="s">
+        <v>196</v>
+      </c>
+      <c r="C62" t="s">
         <v>202</v>
       </c>
-      <c r="B62" t="s">
-        <v>197</v>
-      </c>
-      <c r="C62" t="s">
+      <c r="D62" s="1" t="s">
         <v>203</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
+        <v>204</v>
+      </c>
+      <c r="B63" t="s">
+        <v>147</v>
+      </c>
+      <c r="C63" t="s">
         <v>205</v>
       </c>
-      <c r="B63" t="s">
-        <v>148</v>
-      </c>
-      <c r="C63" t="s">
+      <c r="D63" s="1" t="s">
         <v>206</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
+        <v>207</v>
+      </c>
+      <c r="B64" t="s">
+        <v>190</v>
+      </c>
+      <c r="C64" t="s">
         <v>208</v>
       </c>
-      <c r="B64" t="s">
-        <v>191</v>
-      </c>
-      <c r="C64" t="s">
+      <c r="D64" s="1" t="s">
         <v>209</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
+        <v>210</v>
+      </c>
+      <c r="B65" t="s">
+        <v>193</v>
+      </c>
+      <c r="C65" t="s">
         <v>211</v>
       </c>
-      <c r="B65" t="s">
-        <v>194</v>
-      </c>
-      <c r="C65" t="s">
+      <c r="D65" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="D65" s="1" t="s">
-        <v>213</v>
+      <c r="E65" s="2" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
+        <v>213</v>
+      </c>
+      <c r="B66" t="s">
+        <v>193</v>
+      </c>
+      <c r="C66" t="s">
         <v>214</v>
       </c>
-      <c r="B66" t="s">
-        <v>194</v>
-      </c>
-      <c r="C66" t="s">
+      <c r="D66" s="1" t="s">
         <v>215</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
+        <v>216</v>
+      </c>
+      <c r="B67" t="s">
+        <v>181</v>
+      </c>
+      <c r="C67" t="s">
         <v>217</v>
       </c>
-      <c r="B67" t="s">
-        <v>182</v>
-      </c>
-      <c r="C67" t="s">
+      <c r="D67" s="1" t="s">
         <v>218</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B68" t="s">
         <v>114</v>
       </c>
       <c r="C68" t="s">
+        <v>220</v>
+      </c>
+      <c r="D68" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B69" t="s">
         <v>114</v>
       </c>
       <c r="C69" t="s">
+        <v>223</v>
+      </c>
+      <c r="D69" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B70" t="s">
         <v>114</v>
       </c>
       <c r="C70" t="s">
+        <v>226</v>
+      </c>
+      <c r="D70" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="D70" s="1" t="s">
-        <v>228</v>
-      </c>
       <c r="F70" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed : rename history to evolution
</commit_message>
<xml_diff>
--- a/public/data/db_source/institution.xlsx
+++ b/public/data/db_source/institution.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bassim/code/datannur/datannur_dev/public/data/db_source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96EF1ED4-61DA-4F4F-8F21-D3E4F92036F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E492E9A9-73B3-294C-82B2-3F3C6DDAE1CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2940" yWindow="500" windowWidth="25860" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -710,49 +710,49 @@
     <t>AVASAD : Association vaudoise d'aide et de soins à domicile</t>
   </si>
   <si>
+    <t>profa</t>
+  </si>
+  <si>
+    <t>Fondation PROFA</t>
+  </si>
+  <si>
+    <t>Présente dans tout le canton de Vaud, la Fondation PROFA contribue au développement de la qualité de la vie affective, relationnelle et sexuelle de toutes les personnes, à chaque étape de leur vie.</t>
+  </si>
+  <si>
+    <t>unil</t>
+  </si>
+  <si>
+    <t>UNIL : Université de Lausanne</t>
+  </si>
+  <si>
+    <t>L’Université de Lausanne (UNIL) est une université située dans la campagne de Dorigny, dans le canton de Vaud, en Suisse. Environ 2 300 enseignants et chercheurs ainsi que 950 collaborateurs administratifs et techniques assurent la bonne marche de l'institution qui compte plus de 17 000 étudiants provenant de plus de 86 pays.</t>
+  </si>
+  <si>
+    <t>tag_ids</t>
+  </si>
+  <si>
+    <t>doc_ids</t>
+  </si>
+  <si>
+    <t>pop_com_1</t>
+  </si>
+  <si>
+    <t>pdf_wiki</t>
+  </si>
+  <si>
+    <t>population, societe, transport</t>
+  </si>
+  <si>
+    <t>021 692 11 11</t>
+  </si>
+  <si>
+    <t>L’Office cantonal de la statistique assure l’information statistique en mettant à disposition des autorités, du public et de la collectivité dans son ensemble des informations statistiques pertinentes, fiables et cohérentes.</t>
+  </si>
+  <si>
+    <t>test@email.ch</t>
+  </si>
+  <si>
     <t>Le dispositif de l’AVASAD constitue la plus grande structure parapublique et le principal acteur de l’aide et des soins à domicile et de la santé communautaire dans le canton de Vaud. Le Canton et les Communes pilotent ce dispositif sur la base d’une politique concertée et d’une vision partagée du développement du maintien à domicile.</t>
-  </si>
-  <si>
-    <t>profa</t>
-  </si>
-  <si>
-    <t>Fondation PROFA</t>
-  </si>
-  <si>
-    <t>Présente dans tout le canton de Vaud, la Fondation PROFA contribue au développement de la qualité de la vie affective, relationnelle et sexuelle de toutes les personnes, à chaque étape de leur vie.</t>
-  </si>
-  <si>
-    <t>unil</t>
-  </si>
-  <si>
-    <t>UNIL : Université de Lausanne</t>
-  </si>
-  <si>
-    <t>L’Université de Lausanne (UNIL) est une université située dans la campagne de Dorigny, dans le canton de Vaud, en Suisse. Environ 2 300 enseignants et chercheurs ainsi que 950 collaborateurs administratifs et techniques assurent la bonne marche de l'institution qui compte plus de 17 000 étudiants provenant de plus de 86 pays.</t>
-  </si>
-  <si>
-    <t>tag_ids</t>
-  </si>
-  <si>
-    <t>doc_ids</t>
-  </si>
-  <si>
-    <t>pop_com_1</t>
-  </si>
-  <si>
-    <t>pdf_wiki</t>
-  </si>
-  <si>
-    <t>population, societe, transport</t>
-  </si>
-  <si>
-    <t>021 692 11 11</t>
-  </si>
-  <si>
-    <t>L’Office cantonal de la statistique assure l’information statistique en mettant à disposition des autorités, du public et de la collectivité dans son ensemble des informations statistiques pertinentes, fiables et cohérentes.</t>
-  </si>
-  <si>
-    <t>test@email.ch</t>
   </si>
 </sst>
 </file>
@@ -788,12 +788,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1141,7 +1140,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="C51" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E67" sqref="E67"/>
+      <selection pane="bottomRight" activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1176,10 +1175,10 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>227</v>
+      </c>
+      <c r="H1" t="s">
         <v>228</v>
-      </c>
-      <c r="H1" t="s">
-        <v>229</v>
       </c>
       <c r="I1" s="1"/>
     </row>
@@ -1194,7 +1193,7 @@
         <v>8</v>
       </c>
       <c r="H2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1503,10 +1502,10 @@
         <v>75</v>
       </c>
       <c r="G23" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H23" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1739,7 +1738,7 @@
         <v>125</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E39" t="s">
         <v>126</v>
@@ -2132,8 +2131,8 @@
       <c r="D65" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="E65" s="2" t="s">
-        <v>235</v>
+      <c r="E65" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2175,38 +2174,38 @@
         <v>220</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>221</v>
+        <v>235</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B69" t="s">
         <v>114</v>
       </c>
       <c r="C69" t="s">
+        <v>222</v>
+      </c>
+      <c r="D69" s="1" t="s">
         <v>223</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B70" t="s">
         <v>114</v>
       </c>
       <c r="C70" t="s">
+        <v>225</v>
+      </c>
+      <c r="D70" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="D70" s="1" t="s">
-        <v>227</v>
-      </c>
       <c r="F70" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>